<commit_message>
fix #ner with examples
</commit_message>
<xml_diff>
--- a/analisis_ficheros_ns_v1.2.xlsx
+++ b/analisis_ficheros_ns_v1.2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigBoy\Desktop\nlp-berto-doclass\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BigBoy\Desktop\nlp-berto-doclass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716167F2-D539-4E8D-9323-19EFBEC32364}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB524D6-9460-47D1-89ED-BC9E13BF3DDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1067,7 +1067,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1117,11 +1117,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1851,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -1862,8 +1865,8 @@
     <col min="3" max="3" width="81.109375" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.77734375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" style="15" bestFit="1" customWidth="1"/>
     <col min="8" max="1024" width="12" style="12"/>
     <col min="1025" max="16384" width="12" style="13"/>
   </cols>
@@ -1884,10 +1887,10 @@
       <c r="E1" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2227,8 +2230,8 @@
       <c r="E25" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
@@ -2868,7 +2871,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>53</v>
       </c>
@@ -2882,12 +2885,12 @@
       <c r="E72" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="F72" s="17" t="s">
+      <c r="F72" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="G72" s="17"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G72" s="19"/>
+    </row>
+    <row r="73" spans="1:7" ht="52.2" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
         <v>203</v>
       </c>
@@ -2901,12 +2904,12 @@
       <c r="E73" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="F73" s="17" t="s">
+      <c r="F73" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="G73" s="17"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G73" s="19"/>
+    </row>
+    <row r="74" spans="1:7" ht="52.2" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
         <v>203</v>
       </c>
@@ -2920,12 +2923,12 @@
       <c r="E74" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="F74" s="17" t="s">
+      <c r="F74" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="G74" s="17"/>
-    </row>
-    <row r="75" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="G74" s="19"/>
+    </row>
+    <row r="75" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>53</v>
       </c>
@@ -2941,14 +2944,14 @@
       <c r="E75" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="F75" s="12" t="s">
+      <c r="F75" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="G75" s="14" t="s">
+      <c r="G75" s="15" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>53</v>
       </c>
@@ -2964,10 +2967,10 @@
       <c r="E76" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F76" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="G76" s="17" t="s">
+      <c r="G76" s="19" t="s">
         <v>230</v>
       </c>
     </row>
@@ -2987,11 +2990,11 @@
       <c r="E77" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="F77" s="12" t="s">
+      <c r="F77" s="22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>53</v>
       </c>
@@ -3007,11 +3010,11 @@
       <c r="E78" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="F78" s="12" t="s">
+      <c r="F78" s="22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="87" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
         <v>53</v>
       </c>
@@ -3027,14 +3030,14 @@
       <c r="E79" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="F79" s="12" t="s">
+      <c r="F79" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="G79" s="17" t="s">
+      <c r="G79" s="19" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="87" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>53</v>
       </c>
@@ -3050,14 +3053,14 @@
       <c r="E80" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="F80" s="12" t="s">
+      <c r="F80" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="G80" s="17" t="s">
+      <c r="G80" s="19" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="87" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
         <v>53</v>
       </c>
@@ -3073,14 +3076,14 @@
       <c r="E81" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="F81" s="21" t="s">
+      <c r="F81" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="G81" s="17" t="s">
+      <c r="G81" s="19" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
         <v>53</v>
       </c>
@@ -3090,13 +3093,13 @@
       <c r="C82" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="D82" s="22" t="s">
+      <c r="D82" s="21" t="s">
         <v>225</v>
       </c>
       <c r="E82" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F82" s="22" t="s">
         <v>216</v>
       </c>
     </row>
@@ -3116,11 +3119,11 @@
       <c r="E83" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="F83" s="12" t="s">
+      <c r="F83" s="22" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="104.4" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
         <v>53</v>
       </c>
@@ -3136,14 +3139,14 @@
       <c r="E84" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="F84" s="21" t="s">
+      <c r="F84" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="G84" s="17" t="s">
+      <c r="G84" s="19" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="121.8" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>53</v>
       </c>
@@ -3157,10 +3160,10 @@
       <c r="E85" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="F85" s="17" t="s">
+      <c r="F85" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="G85" s="17" t="s">
+      <c r="G85" s="19" t="s">
         <v>254</v>
       </c>
     </row>
@@ -3180,11 +3183,11 @@
       <c r="E86" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="F86" s="12" t="s">
+      <c r="F86" s="22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>100</v>
       </c>
@@ -3200,14 +3203,14 @@
       <c r="E87" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="F87" s="12" t="s">
+      <c r="F87" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="G87" s="14" t="s">
+      <c r="G87" s="15" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
         <v>100</v>
       </c>
@@ -3223,11 +3226,11 @@
       <c r="E88" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F88" s="17" t="s">
+      <c r="F88" s="19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
         <v>100</v>
       </c>
@@ -3243,11 +3246,11 @@
       <c r="E89" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F89" s="17" t="s">
+      <c r="F89" s="19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>100</v>
       </c>
@@ -3263,11 +3266,11 @@
       <c r="E90" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F90" s="17" t="s">
+      <c r="F90" s="19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
         <v>100</v>
       </c>
@@ -3283,11 +3286,11 @@
       <c r="E91" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F91" s="17" t="s">
+      <c r="F91" s="19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
         <v>100</v>
       </c>
@@ -3303,11 +3306,11 @@
       <c r="E92" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="F92" s="17" t="s">
+      <c r="F92" s="19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A93" s="14" t="s">
         <v>100</v>
       </c>
@@ -3323,11 +3326,11 @@
       <c r="E93" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F93" s="17" t="s">
+      <c r="F93" s="19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
         <v>100</v>
       </c>
@@ -3343,11 +3346,11 @@
       <c r="E94" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F94" s="17" t="s">
+      <c r="F94" s="19" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="52.2" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
         <v>196</v>
       </c>
@@ -3363,14 +3366,14 @@
       <c r="E95" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="F95" s="12" t="s">
+      <c r="F95" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="G95" s="14" t="s">
+      <c r="G95" s="15" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="52.2" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
         <v>196</v>
       </c>
@@ -3386,14 +3389,14 @@
       <c r="E96" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="F96" s="12" t="s">
+      <c r="F96" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="G96" s="14" t="s">
+      <c r="G96" s="15" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="52.2" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>196</v>
       </c>
@@ -3409,14 +3412,14 @@
       <c r="E97" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="F97" s="12" t="s">
+      <c r="F97" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="G97" s="14" t="s">
+      <c r="G97" s="15" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>203</v>
       </c>
@@ -3432,11 +3435,11 @@
       <c r="E98" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="F98" s="12" t="s">
+      <c r="F98" s="22" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="348" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>203</v>
       </c>
@@ -3452,14 +3455,14 @@
       <c r="E99" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="F99" s="17" t="s">
+      <c r="F99" s="19" t="s">
         <v>288</v>
       </c>
-      <c r="G99" s="17" t="s">
+      <c r="G99" s="19" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="174" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
         <v>203</v>
       </c>
@@ -3475,10 +3478,10 @@
       <c r="E100" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="F100" s="17" t="s">
+      <c r="F100" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="G100" s="17" t="s">
+      <c r="G100" s="19" t="s">
         <v>293</v>
       </c>
     </row>

</xml_diff>